<commit_message>
Get daily reddit data: Tue Sep 24 08:11:18 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_29.xlsx
+++ b/data/collected_data/2024_09_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C486"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3151 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1fo71hk</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use tip extensions with BIAB? </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fo71hk/can_you_use_tip_extensions_with_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1fo6o5i</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>My nails :)</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l9onxjugjpqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1fo5pjg</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Past two sets!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo5pjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1fo5o8u</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>botched nail job</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fo5o8u/botched_nail_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1fo539x</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Firts time putting fake nails ^^</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo539x</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1fo4yb0</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>design i came up with</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo4yb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1fo4mry</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">one of my personal favorites </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfd2v708uoqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1fo3tl6</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short and tinted baby pink </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pusa004loqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1fo3b33</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>I actually like the way matte glitter looks</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo3b33</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1fo2y7o</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t keep color on for more than 24 hours </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo2y7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1fo2x84</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>What should I add to this sparkly base?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45qm8u90coqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1fo28rr</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>These are about a week old so they're a little worse for the wear, but I like them!</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo28rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1fo1yup</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llzarpn33oqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1fo1sxi</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>French tip dip mani. Normal?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo1sxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1fo1rz1</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>nail charms</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fo1rz1/nail_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1fo1qye</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>🕸🩷👻</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo1qye</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1fnzyjv</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Took this right before I lost my thumb nail 🥲</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9svngu2mknqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1fnzu8v</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just started getting back into nails. </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnzu8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1fnz4aa</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>hyperrealistic natural bone nails</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnz4aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1fnzjye</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Chocolate milk 🐮🥛</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnzjye</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1fnzgfl</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>What do you guys think? Only been painting/getting my nails done for a year. 2nd ever professional job.</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fo3pnui3gnqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1fnze0e</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>🍁🌺🌿</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfp55zqgfnqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1fnz6pi</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver chrome with black rhinestones </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ov7zxh9qdnqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1fnyeu2</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Struggling to find gel tips that fit my big thumbs lol</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnyeu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1fnylgl</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Gel Nails - tips?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoarb1hn8nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1fnyq8e</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Some of my 2024 sets 💖</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnyq8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1fny8eb</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make builder gel last? </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fny8eb/how_to_make_builder_gel_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1fnxwiv</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>What am i doing wrong?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnxwiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1fnxvmw</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Natural” xxl stilettos </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnxvmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1fnxrkv</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Are gel nails suppose to peel off?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnxrkv/are_gel_nails_suppose_to_peel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1fnxklk</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don't usually like purple but that polish changed my mind i guess!! 🫶🏻 </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qgaakc00nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1fnxdyp</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>@Klawsbysophia on ig</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jq44c1jymqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1fnwsyc</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>What color and shape should I get? I feel like this design makes my fingers look more awkward. My natural nail beds are wide and short and my index and a middle finger point outwards. I'm not sure what to do with them.</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnwsyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1fnvs7p</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Press on nails Reusability.</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnvs7p/press_on_nails_reusability/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1fnx5z6</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shorties bubble chrome nails </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3vttz2pwmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1fnx1ee</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Is putting nail polish/Lacquer in the fridge good for the polish?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnx1ee/is_putting_nail_polishlacquer_in_the_fridge_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1fnwjts</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Do you like accessories in your manicure? I feel them a little annoyed 🫣</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwgn30asrmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1fnwjoc</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Fall Season = Sultry + Spooky</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnwjoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1fnwhn0</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Mrs. Potts and Chip 🥰😍🫖☕</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chb6pvz9rmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1fnvjvn</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of Nails! </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18qk8y7zjmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1fnv548</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Top white part of my nail tore off when I was removing fake nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnv548/top_white_part_of_my_nail_tore_off_when_i_was/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1fnukyx</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this normal? </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnukyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1fnv26d</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Cherry red 🥰</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snliom3agmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1fnu9mc</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Recovering from gel allergy</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnu9mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1fnu6hd</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn nails </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnojmslp9mqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1fntq14</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Keep being told it's too early </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99u9oh9c6mqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1fntpem</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard gel on natural nails </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fntpem</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1fntoxx</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Color match?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry2ti2y36mqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1fnth09</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make cuticles healthy because now they look like this… </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnth09</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1fntd9w</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Halloween is coming</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fntd9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1fntd7x</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Neon for summer</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fntd7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1fnsbay</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">September nails </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m87bswczvlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1fnrmnb</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>White Gel</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnrmnb/white_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1fnqr3w</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my first full set of gel-x (american pose) </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnqr3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1fns3g7</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did 2 layers of magnetics. </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z8cn9bydulqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1fns2ye</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>press ons</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fns2ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1fnrw2w</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>a set from today🐍🦇🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnrw2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1fnrumy</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven't posted I. A while but these turned out too beautiful to not share !! </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8wy6nkrkslqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1fnrut8</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Just starting out</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnrut8</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1fnrn0p</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Faking a natural nail? </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41kfxnk2rlqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1fnrks3</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Koi fish nails</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1q0hxomqlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1fnrh9p</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>New🎀💖</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnrh9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1fnrglv</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vacation nails </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tlcwcorplqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1fnr9w2</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Homemade French Tips </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tsp3o0folqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1fnr3gk</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Sometimes you just have to mix some polishes together to get the perfect colour 💅🏻</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnr3gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1fnqm3t</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Miffy nails 🤍</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppmv5utljlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1fnqis2</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Pretty Duck Nails</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnqis2</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1fnqbsv</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do i have enough space for a fill? </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx8wb3eihlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1fnq9of</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Feeling purple lately</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gc7u8n2hlqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1fnq770</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>this colour never disappoints</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxy010ckglqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1fnpr4l</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Loving the green and gold right now</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnpr4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1fnpayw</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with the length 🍒 </t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnpayw</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1fnox85</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Don't book Friday the 13th!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnox85</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1fnorqe</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Sets I’ve Had</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnorqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1fnozfg</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Hate my gel color any options without removal ?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnozfg/hate_my_gel_color_any_options_without_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1fnoyyo</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Is it good ombre?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnoyyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1fnohcr</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>In love with this set I recently got done. This is only my third time ever getting my nails done and I am ✨obsessed✨</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnohcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1fno3av</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Pretty nails with my cute hampter💅</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fno3av</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1fnnyp8</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My most recent nail sets, I’m pretty new to press ons </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnnyp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1fnn1p6</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Does anyone else use seasonal color analysis to choose nail polish colors?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnn1p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1fnmyma</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I have recently started free handing my fake nails... what do you think?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnmyma</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1fngpvm</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>How do I fix my nails after years of biting them?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fngpvm/how_do_i_fix_my_nails_after_years_of_biting_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1fnjwo6</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>why did my nails change color</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnjwo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1fnjwze</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>First time doing acrylics</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7h6m0g5y4kqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1fnhf9x</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I did a refill on my grown nails. How bad is it be honest 😂</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnhf9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1fnh86n</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Newbie Questions about Starting</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnh86n/newbie_questions_about_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1fnmo2o</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Press Ons!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnmo2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1fnm39r</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>White is my new favourite color!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnm39r</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1fnlymd</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian Manicure </t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnlymd</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1fnlrv0</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Studio Ghibli nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8u2trwjzjkqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1fnllhe</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Say meow 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmil6u1kikqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1fnljr9</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Comic ones 👀</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp3f89u6ikqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1fnlhet</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Hell girl thumb I made ✨</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbhs0cnohkqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1fnlfr7</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Really loving Chrome on French lately 😇</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnlfr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1fnley1</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>What do you guys think about my harness press-on nails?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikmvdde5hkqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1fnl0ak</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do my press one look? </t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn9ihxc1ekqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1fnkpgs</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Obsessed with these 🎀</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mufgi7mkbkqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1fnkju1</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>A woman with her nails done doesn't want war with anyone!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aija3aj3akqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1fnk3cw</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Good stores to buy at?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fnk3cw/good_stores_to_buy_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1fnjal9</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new(ish) ✨✨ </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnjal9</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1fo79tz</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not My Finest Paint Job But I Love The Way They Came Out </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl3y7c2srpqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1fo6g8b</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>What does my girlfriend need to do to make her nails last longer? They keep breaking.</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fo6g8b/what_does_my_girlfriend_need_to_do_to_make_her/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1fo6aj5</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First casualty after 3 months of nail growth. </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo6aj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1fo5lb2</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Super happy with how my nails look now vs when I first started</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo5lb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1fo3jm2</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>LynB really does blurples well 🌙⭐️</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo3jm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1fo2v80</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Midnight in Moscow for fall </t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fo2v80/midnight_in_moscow_for_fall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1fo2gqv</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>New to nail art and my experiment turned into me creating slime nails</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo2gqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1fo2anl</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>nostalgia by death valley nails 🐚</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2v33uy46oqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1fo1d4y</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Joie de Vivre</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo1d4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1fo0lsx</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is your go to basecoat for preve ting staining and yellowing? </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fo0lsx/what_is_your_go_to_basecoat_for_preve_ting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1fo07ci</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Canmake Colorful Nails- N08 Misty Mauve</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmq2harumnqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1fo01wb</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>It's Fall, Y'all!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nz59jltglnqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1fnzl9p</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven't done my nails in a while but I'm pleased 🙏 </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l9h7oi9hnqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1fnyvl3</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$3 polish Glass Ceiling by Pop Aarazzi </t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qptkws51bnqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1fnyqyi</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Halloween Starts Now</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fce0drw9nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1fnyje4</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>What Kind of Manicure Did I Get?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnyje4/what_kind_of_manicure_did_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1fnydkh</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>First attempt at tie-dye nails!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3gloz9p6nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1fnyb7q</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Mooncat Enchanted Mist</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9umosn56nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1fny9fk</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>✨ Prism Parade's Alchemy Collection</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fny9fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1fny8r5</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Anyone buying the new mooncat collection?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fny8r5/anyone_buying_the_new_mooncat_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1fny03w</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Glitter tipped manicure polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fny03w/glitter_tipped_manicure_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1fnxtpn</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Matte flakies are the best flakies!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5me666p32nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1fnwljj</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this bright blue </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5eajxe3smqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1fnw6qs</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Polish changing color after topcoat?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnw6qs/polish_changing_color_after_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1fnvq1w</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>LynB Designs - Sagittarius (The Archer) 🏹</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycwb7dhalmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1fnvbmz</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m desperate </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnvbmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1fnv6f7</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super hard top coat recommendations </t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnv6f7/super_hard_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1fnuw9w</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>The one and only 💜💜</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnuw9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1fnu8gq</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Posting my last summer many</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnu8gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1fntzq3</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Recommendations for a budget-friendly, milky light pink nude?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fntzq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1fntud2</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Dupe request for WFL Frog &amp; Toad</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fntud2/dupe_request_for_wfl_frog_toad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1fntmzb</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Color match?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibjmjyep5mqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1fntgro</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can't stop staring at my nails now HELP </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fntgro</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1fntgbp</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>ILNP - Bitten</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fntgbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1fnsa6p</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal is a love hate relationship </t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnsa6p/thermal_is_a_love_hate_relationship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1fns4s5</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>made this set to match my latest obsession with snake print 🐍</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fns4s5</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1fns0r7</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>ILNP does it again! 🖤💜</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bjj6fcvtlqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1fnrqm3</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>No bubbles</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vgbqgbsrlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1fnrodz</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>More dark polish on short nails!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnrodz</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1fnr87z</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Homemade French Tips 💅</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkroyo92olqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1fnr6ze</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Wanted something whimsical cuz I got a bad case of the Mondays</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnr6ze</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1fnr4d9</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Mooncat Illusionist on shorties</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfymi6x9nlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1fnr0vk</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>LynB Desisns - Athymy</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yud13okimlqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1fnr0kq</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Me: you know those snicker bar veins? Them: say no more </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x70saakhmlqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1fnqhly</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>How to strengthen my long nails?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnqhly/how_to_strengthen_my_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1fnqgxz</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>not sure where I was going with this 🫣</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnqgxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1fnq5u2</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Holo Taco Ivy League is a perfect fall transition color</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnq5u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1fnpm08</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Any chance I'll ever get my hands on Ethereal Lacquer: Lorraine?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnpm08/any_chance_ill_ever_get_my_hands_on_ethereal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1fnp7rg</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Boop The Snoot in the Land of Lava... Also... Opinions on Vibrant Scents WET &amp; HARD PLEASE?! </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jh9dgbzg9lqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1fnolvi</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>6 week growth progress after a life long nail chewing habit</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ewl5yl05lqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1fnnywp</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>💛Yellow There💚</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnnywp</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1fnnwv5</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Peel off base coats (specifically Orly One Night Stand)</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnnwv5/peel_off_base_coats_specifically_orly_one_night/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1fnmo64</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layering some favorites = new favorite </t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i3n8r9asqkqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1fnmkog</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Time for fall nails! ✨️🪲</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnmkog</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1fnm2zb</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s fall!! 🍂 </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnm2zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1fnl7yt</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Aurora Borealis by Whatcha (PPU Dec/23)</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnl7yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1fnl7aj</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>lowkey matching 🤩</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3gco0xhfkqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1fnkmc6</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my hands on Essies "Multifaceted" </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnkmc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1fnk3vh</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Essie fab florals</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnk3vh</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1fnk184</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>🍃Birch Please 2.0🍃</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnk184</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1fnjq8n</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>🎶 I’m an excavator- Hey, dirt, see you later! 🎶🏗️</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7rnh4hd3kqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1fnjin8</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Monday Morning Multichrome!</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byx60hzg1kqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1fnjimp</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I asked for vs. what I got </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnjimp</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1fnj5a2</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Seche vite isn't very fast</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t81hgvh7yjqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1fnioty</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has mooncat fixed their bottles yet? </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fnioty/has_mooncat_fixed_their_bottles_yet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1fni22l</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Did my first magnetic mani 🤩</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y5kssphbnjqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1fngtvj</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fngtvj/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1fo37c0</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>16 hours of painting. Worth every minute in my eyes. Now for a little spa time as I put them on. Click to see all 10!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo37c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1fo2l9g</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Moodeng portrait</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xj1a6mju8oqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1fo2ca7</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>SpongeBob nails 🍍</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mc9k69k6oqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1fo1u4n</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Can someone try this nail design?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g04dws2w1oqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1fo15yj</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>did my nails and toes to match #beginnernailart</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo15yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1fnzzr4</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Spooky Season</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnzzr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1fnxqwy</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Non- dominant hand… I tried!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy2swzeg1nqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1fnx3vl</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tufted Nails </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4axb3778wmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1fnv5nv</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anaranjado y negro </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnv5nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1fnuo5z</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>News Nails 💅😍</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnx9lpjbdmqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1fnuauk</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧡🖤 </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qokgvqdlamqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1fnt4bg</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>French Red 💋</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky0gqbhv1mqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1fnsvft</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>What is this type of brush called?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnsvft</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1fnqryt</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I haven't done my nails in awhile but I think these came out cute! Beginner nail artist 💕</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnqryt</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1fnpoxn</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Dazzling colour purple</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnpoxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1fnotp2</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Client requested a Día de muertos Freestyle ✨🧡</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnotp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1fnnlv0</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>It nails with both Clowns</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fnnlv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1fnhply</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Client’s vision came true🙂‍↕️😆</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o95g30rbjjqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Sep 25 08:10:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_29.xlsx
+++ b/data/collected_data/2024_09_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C486"/>
+  <dimension ref="A1:C673"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8695,6 +8695,3185 @@
         </is>
       </c>
     </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1foysz6</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>My friend is becoming a nail tech!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foysz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1foyp7k</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Sweater weather</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ionvspc0qwqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1foy8n1</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kokoist help! </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1foy8n1/kokoist_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1foy3so</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Thanks u/KneemaToad for the inspo - took your “mistake” and put a Halloween spin on the colours</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb3ghvq3iwqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1foxzx6</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Next Level</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foxzx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1foxpdz</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding nails for tomorrow. </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yht0knjvcwqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1foxatp</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I’m obsessed! 💕</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpbeiqqp7wqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1fovx6f</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>first time!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fr0aumrrvqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1fovmdp</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>simple red press ons ❣️</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ksqaukvmovqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1fovenw</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>i absolutely love this shade 😍</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qpr6q0dmvqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1fouj5b</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just found this set I had a while ago in my pics and thought I’d share, because I absolutely loved them </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cltea9qqdvqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1fou2gd</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Ready for fall!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5anxg1yg9vqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1fotu1t</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fotu1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1fotkkd</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>My red nails 🥵</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buznd9ir4vqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1fotaif</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>I did my own gel nails for the first time 🤭</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fotaif</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1fot4s9</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good nail glues? </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fot4s9/good_nail_glues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1fosn1z</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>✨🌙 sparkly star and moon set ✨🌙</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76niima9wuqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1fosjwu</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I’m looking for the impossible</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x085n0gvuqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1fosj1e</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> XXL Stiletto’s 🕷️🕸️ Polygel Edition💅</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x895ef97vuqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1fose4t</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: first day vs second day, did I make it worse or better? </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fose4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1fos8q9</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🖤 </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/694z49ynsuqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1forw4r</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Can I trust lanailsupplies.com</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.lanailsupplies.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1for1mh</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>What I got vs what I asked for, inspo from nailandinklove.com</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1for1mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1fortju</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Green &amp; Gold Glamour</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npyvg7juouqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1forn8h</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Ready for fall with tortoise shell nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1forn8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1forhyy</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any fans of The Shining? </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9749t9zluqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1forhwv</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New fall set on a client! Whatcha think!? </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cy2zrskyluqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1for38p</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>My daughter asked for press-ons....this is what I delivered</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1for38p/my_daughter_asked_for_pressonsthis_is_what_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1foqp08</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I get gel manicure with ring of fire on nails? </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1foqp08/can_i_get_gel_manicure_with_ring_of_fire_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1foqldi</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>First BIAB and in love</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foqldi</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1foql49</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brat nails for the concert </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foql49</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1fopwot</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>New to nail painting, advice needed</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fopwot</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1fopq5y</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>probably the best ones i ever got</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fopq5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1fopnp8</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>I'm in love ❤️</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bsnsfk116uqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1fop8n2</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Lovee my new set 😍✨</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6bw6dcj2uqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1fop7vb</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Just bought supplies to do my own press-ons! Is this all the nail prep/things I need?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhk7gwzc2uqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1fooir0</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Will press ons fit men?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fooir0/will_press_ons_fit_men/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1fooigr</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Played around with gem placements for these pressies🍷✨</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fooigr</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1foogfq</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Did these simple Halloween nails on myself!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foogfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1foo8ei</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think this is going to be my nail tech for a really long time </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vowfcdcutqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1fons86</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maybe regretting this brown </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvy1e28vqtqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1fonopm</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Cherry mocha 🍒</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fonopm</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1fonkit</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Every day they come out better or what?😮 </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tusfrmq8ptqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1fond6z</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Long nails as a closeted trans girl</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fond6z/long_nails_as_a_closeted_trans_girl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1fommqc</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Find the color?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t2uz876itqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1fomiuv</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you guys get nervous when your toenails get drilled? </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fomiuv/do_you_guys_get_nervous_when_your_toenails_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1fomik0</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Some Country Nails</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fomik0</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1fomej5</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Milky almonds🤍</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqknkatfgtqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1fom8zu</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz4pafz8ftqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1fom69g</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Little hearts!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fom69g</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1foltcp</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Finally growing, no color.</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/za2ux1z1ctqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1fok9c9</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Why does this happen every time I do my nails?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fok9c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1follxb</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Help with shape!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1follxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1folglk</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>I hate green but my bf begged me 😭😭</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw0hdjde9tqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1fol1ic</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Currently obsessed with doing magnetic gel at home</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihxp70tb6tqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1fokrnt</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Halloween</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fokrnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1fokkwb</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>I fell in love with my nails!!</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlanckb03tqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1fok67c</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>I got a mystery gel manicure today</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fok67c</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1fojw5b</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Medieval vibes.</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9o28vcwxsqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1fok14g</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Mini gemstones and magnetic polish</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8dx2j8xysqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1fojmkx</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Last “summer” set. Going into fall colors on my next set 🍁</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w48mafrzvsqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1foibsj</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Pink chrome 🌸</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foibsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1foiznq</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Any luck with press on nails and if so do you have any recommendations?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1foiznq/any_luck_with_press_on_nails_and_if_so_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1fojbkm</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>My finger nail fell off! Help!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fojbkm/my_finger_nail_fell_off_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1foj2vd</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Just a little tortoise shell moment☺️</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foj2vd</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1foiwah</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>First nail art!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quwsuoplqsqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1foiito</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>lil halloween 🩸drip 🩸</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foiito</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1fohsb6</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Nail Art Supplies?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fohsb6/nail_art_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1foi1me</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Happy belated fall equinox! ♥</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpkd4608ksqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1foi0au</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>🌿 My long natural nails before and after painting 🌿</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cremn732ksqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1fohi8c</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>OPI Natural Nail Strengthener</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fohi8c/opi_natural_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1fohbh9</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Anyone ever find glue got press ons that makes them last? I love a good press on set but hate when they pop off after a day!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mh5oe6s0fsqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1foh2v3</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Spooky Season👻</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1xtkv79dsqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1fogzzi</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Biab nails when swimming &amp; sauna regularly.</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fogzzi/biab_nails_when_swimming_sauna_regularly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1fogi54</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sharing because I'm the most proud of this set! </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fogi54</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1foghby</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Red chrome with pink hearts &amp; stars</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/intpn37o8sqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1fogbvb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>What's the goal of cutting/pushing back the cuticles?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fogbvb/whats_the_goal_of_cuttingpushing_back_the_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1fofo4y</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Did the nail tech I went to shave my nails down too much?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o26huxq2sqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1fodagg</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ever nails done by a nail stylist  </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fodagg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1fofd9t</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I liked the blue </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7kj6lhh0sqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1foes5h</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Love extra nails ✨🖤🫶🏼❤️</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foes5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1fodz5t</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French tips on natural nails </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eey0uzv0qrqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1fodggb</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Manly shit right here. 💅</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fodggb</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1focxan</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Magnetic pedicure</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id7czbyshrqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1focchd</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Fall ✨️🍁</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1focchd</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1focakw</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these on a client! Watcha think!? </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvfuou4mcrqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1foc8jn</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>New fall nails, gold and silver</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv7w2t15crqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1fobaa8</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>I am so obsessed with these little shroomies</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygc6mc4t3rqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1fob0tn</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>finally figured out how to do isolated chrome!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fob0tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1foauns</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Still not over my summer nails 🍋💛</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foauns</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1foahws</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Dark green nails</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd1i5usdwqqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1fo9r70</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>do we like this??</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bjv5r8eoqqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1fo8lfw</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>I have finally finished the beetlejuice nail set!😆💕 These are 10XL nail tips and not to be worn daily I just made them for fun ☺️</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo8lfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1fo8iie</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>a good nail glue for press on?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fo8iie/a_good_nail_glue_for_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1fo7mav</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn vibes </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo7mav</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1foza4y</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Are there any good polish advent calendars this year?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foza4y/are_there_any_good_polish_advent_calendars_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1foyxbj</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Fall nails! 🍂</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foyxbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1fox2hn</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>First time doing gel nails, but I don't like the tip, how can I fix the gel so it doesn't look like that?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fox2hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1foyo6s</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>ILNP {Flower Child}</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foyo6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1foxqys</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Existential crisis (new to doing nails)</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foxqys</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1foxmdd</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>EDM - Rise Again (Sep 2024)</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foxmdd/edm_rise_again_sep_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1foxle8</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Is Cirque Still Selling Skinny Brush Polish?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foxle8/is_cirque_still_selling_skinny_brush_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1fox1bz</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Flicker 🕯️</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02gbrxcg4wqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1fowje8</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>I got this new icy powder</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu4zz2qhyvqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1fofv20</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Find a new salon? Or am I just picky?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fofv20</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1fow6ct</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Great Lake Lacquer recs? </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fow6ct/great_lake_lacquer_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1follrh</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>need inexpensive nail polish recommendations!!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1follrh/need_inexpensive_nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1fovxxq</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Did my nails to match my tortoise Kevin’s :)</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fovxxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1fov0f1</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a dupe of Glowy AF - Rogue Lacquer? </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fov0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1fouvgv</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second post as video, they are growing on me!!! </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d62kak0xgvqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1fou60q</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>FYI Fancy Gloss Restock 9/27 info</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohzh2fcdavqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1fou14v</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Berry for Fall!</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fou14v/berry_for_fall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1fotx8h</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall or ghosts? why not both </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fotx8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1fotrga</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Holo Taco Inkwell</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhg2r8il6vqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1fosw54</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adding to the fall skittles </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fosw54</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1fosfy5</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>This mani makes me feel like a fairy princess</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7nh3qr8duuqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1fosedp</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>i’m rover it by holo taco 🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jmufqj0uuqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1fosc84</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: first day vs second day, did I make it worse or better? </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fosc84</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1fornpk</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I'm putting a layer of glow in the dark under every sheer polish from now on</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fornpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1for457</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Holo Taco stained the SHIT out of my nails. 😱</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1for457</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1fopyyn</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Just getting back into painting my nails after years</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fopyyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1fopwgs</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>✨🪻Heather🪻✨</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik8x89z48uqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1fopuqv</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Hi pumpkin!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1za4agnq7uqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1fopl51</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Ultrashorties Represent</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69y2vngf5uqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1fopibv</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Sad about a big chop? Sparkles help :)</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fopibv</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1foowfh</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reminded me of a blue galaxy </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipxvu7aiztqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1foos32</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>how to get clean looking cuticles</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foos32/how_to_get_clean_looking_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1fooph8</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Sun kissed Spell (thermal + shimmer)</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kuocb5i1ytqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1foojyf</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Chanel lipstick/gloss matching Chanel Pompier nail polish?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foojyf/chanel_lipstickgloss_matching_chanel_pompier_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1foobsm</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Blue chrome nails  with regular nail polish for fall 🍂💙</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud7qwwo2vtqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1foo97w</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>First Glam Polish order on the way!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foo97w/first_glam_polish_order_on_the_way/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1fonxzo</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Dupe for &amp; Other Stories Voilette Gleam?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://imgur.com/BJ79tkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1fonxzg</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>So hard to do justice on film</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fonxzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1fomif0</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>How much thinner am I supposed to add?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fomif0/how_much_thinner_am_i_supposed_to_add/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1folxxc</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>When do you know it’s time to add thinner?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1folxxc/when_do_you_know_its_time_to_add_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1folsw7</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Is it true or false you need to take polish breaks to let your nails breathe?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1folsw7/is_it_true_or_false_you_need_to_take_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1folhha</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Leotia” from Daisy Chain Polish </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1folhha</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1fokmif</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mum has allowed me to do her nails! </t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fokmif/my_mum_has_allowed_me_to_do_her_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1fojz7c</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Can anyone help me ID a dupe for this discontinued H&amp;M Hinterland creme nail polish?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fojz7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1fojvgj</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Dark Academia nails for an IG collab 🖤</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fojvgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1fojdy0</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fojdy0/polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1foi7ea</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>(MAKER) Happy belated fall equinox y'all!! ♥ ♥ ♥</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3zwv40dlsqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1foi15l</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Mysterious Uranus! 🪐</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foi15l</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1fohy20</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>10/10 for Hallucinate</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fohy20</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1fohqkn</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">psilocybin video swatch </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c0731nk1isqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1fohons</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">psilocybin swatches </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fohons</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1fohkp4</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Your heart is a black hole P.2</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fohkp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1fohbuk</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Mooncat Maelstrom</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26ikmmn2fsqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1fog7pd</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe? </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hibamgyr6sqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1fofg07</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An iridescent milky can be good for all seasons </t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fofg07</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1fof8pq</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Obnoxiously Fall Nails!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fof8pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1fof2r4</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No color this time. </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep25p8w9yrqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1fof0o7</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Cashmere</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fof0o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1foek6g</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>favorite nail polish remover/polish remover tips?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1foek6g/favorite_nail_polish_removerpolish_remover_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1foeaau</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Looking for a translucent (non gel) amber polish</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kisxwq2dsrqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1foe8qc</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>If you work in corporate america, how do you decide “the line” for your mani?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foe8qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1fodmth</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Magnetic polish without needing uv/led light?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fodmth/magnetic_polish_without_needing_uvled_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1fod9zh</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Bite Me Sparkle Fangs</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fod9zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1focsfx</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Smokescreen - mooncat</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1focsfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1fobkol</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>2024 nail polish goals - check in</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/s/HdQt2XYOMi</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1fobedd</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I might have to go through my entire magnetics collection before ever switching back to another formula. Thanks horseshoe 🧡💛</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/71iebenn4rqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1foaps4</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Fall skittle 🍁🎃❤️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foaps4</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1fo87uy</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Proximal nail fold?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo87uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1fo8306</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Closest I’ve gotten to a velvet nail, I then immediately dropped it.</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/144jw97b3qqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1fo7kdb</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Help me perfect my polish routine</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fo7kdb/help_me_perfect_my_polish_routine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1fo7ieu</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>How to remove nail glue that spilled and dried off of my table?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fo7ieu/how_to_remove_nail_glue_that_spilled_and_dried/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1fo1fjt</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>My first KBShimmer hauls</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo1fjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1foyolq</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Sweater weather &amp; 3D</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzkhxrvrpwqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1fovgbj</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Hello, Help with my design</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzxarbgumvqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1fouj1v</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>How can one start creating images/stickers like this? What is the printing technique called?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fouj1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1fotv12</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Halloween nail inspo</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fotv12</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1fosbbo</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: first day vs second day…did I make it better or worse? </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fosbbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1fosawm</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">XXL Polygel Stilettos🕷️🕸️ </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qfpbxjh5tuqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1for4jo</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>My daughter asked for press-ons....this is what I delivered</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1for4jo/my_daughter_asked_for_pressonsthis_is_what_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1fopc3l</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Where can I get stamps?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fopc3l/where_can_i_get_stamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1fonymd</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nod to the juice, featuring Sally Hansen X Beetlejuice Collection: Say it 3 Times </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fonymd</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1fonyl3</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Need some ideas!!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fonyl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1fonqb9</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Opinions?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fonqb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1foni5c</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>DnD/Halloween nails. Credit @MuiiBailey</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foni5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1fok5nw</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Alright I put them on!! I can't stop looking at my hands! I'm pleased with how this design turned out! Mountains next!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fok5nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1foi4db</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Happy belated fall equinox! ♥</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6g3cgtruksqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1fofq5q</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying a witchy set </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fofq5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1fof769</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Learning new techniques, how can I improve? (Details inside)</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fof769</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1foeyic</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Aura Nails</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1foeyic</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1focpb7</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>recently finished in a nice burgundy tone</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuo28nz0grqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1fo8l4l</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>I have finally finished the beetlejuice nail set!😆💕 These are 10XL nail tips and not to be worn daily I just made them for fun ☺️</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo8l4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1fo7zzf</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suki waterhouse said my work is incredible!! </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fo7zzf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Sep 26 08:10:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_29.xlsx
+++ b/data/collected_data/2024_09_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C673"/>
+  <dimension ref="A1:C845"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11874,6 +11874,2930 @@
         </is>
       </c>
     </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1fpqmy5</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Builder gel question</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4t4wl1cw3rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1fpqjp6</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>candy corn🎃</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpqjp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1fppmta</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was so proud, and then... </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n10exov0j3rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1fpplqk</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>First Time Doing My Nails All By Myself!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpplqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1fpq1cs</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Autumn is here, which means red szn is here 😈</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpq1cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1fpoauy</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Told myself I'd give my nails a break</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpoauy</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1fpnxtp</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What colour should I do my nails!? This is the dress I will be wearing. (October Wedding) </t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44de3roly2rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1fpn6hz</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Going apple picking on Saturday 🍎</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpn6hz</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1fpmb60</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feedback ! I got my nails done yesterday and there is something about the shape or length I don’t like, but I can’t put my finger on it. Is round the best shape for me or should I try something else? These are my natural nails with luminary and gel polish. </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/729cfy6vh2rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1fpm2fc</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>When you don't know if you love it (diy)</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnfwbqohf2rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1fplzad</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>obsessed 😩</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fplzad</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1fpkjb8</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Why does my gel manicure look really gloopy/dry?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpkjb8/why_does_my_gel_manicure_look_really_gloopydry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1fplhym</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Gilded Galaxy</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fplhym</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1fplgqt</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Question about milky white polish</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fplgqt/question_about_milky_white_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1fplcdn</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best friend did my nails for vacation </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fplcdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1fpkwtb</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fall nails </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpkwtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1fpkdch</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>I think I’m a press-on girl now 🥹🐙</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpkdch</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1fpi4v8</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Really dislike my nails. Did the salon mess up?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0ayf5vjf1rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1fph7mx</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>fumbled and pressed my false nail on crooked</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gqvqqgv71rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1fpgc5n</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>First time getting acrylic! Safe to say I won't be going back 😭</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpgc5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1fpilqk</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>In search of…</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpilqk/in_search_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1fpjiwe</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Love it or not 😉</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtd1pgwsr1rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1fpj323</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>The garden is why my nails will always be chipped. OPI: 15 minutes of flame</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax7zn32wn1rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1fpiue2</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Getting married in less than 3 weeks. Newbie with no idea what to get!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpiue2/getting_married_in_less_than_3_weeks_newbie_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1fpiiaw</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>my fiancé picked me out some nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpiiaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1fpgzaj</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Halloween </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpgzaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1fphko4</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I promise your cuticles will heal with time (and oil) 💚</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fphko4</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1fphoyp</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Love these so much!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fphoyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1fphmwa</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Today’s Set</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1pzzr1db1rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1fph2ud</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally! </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fph2ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1fpg8r9</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was inspired by Nana/Vivienne Westwood 💗 </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2n3tzlzz0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1fpgjnn</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">so happy w this bone color under a matte topcoat </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5exhv1xf21rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1fpg6ry</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Color different from swatch?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpg6ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1fpfsti</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another simple classic fall pink </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vs6240ngw0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1fpfn3t</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Nail Drop</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpfn3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1fpfjux</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails 👻 </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpfjux</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1fpfedd</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbv8bqwdt0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1fpf4s9</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>they’ve grown on me!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpf4s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1fpev8d</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>My wedding nails ✨</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpev8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1fpdrwu</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>First self-acrylic and nail care tip questions!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpdrwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1fpcy45</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Post Acrylic Help</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzdv3xjua0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1fpdzy3</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>I’m obsessed with this color gradient! 😍💅 The transition from nude to brown with the small heart detail is so beautiful 😍</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzbsfr5oi0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1fpdl9g</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>We are fresh 💅</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28k73eeof0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1fpddj4</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail foils! Went well♥ </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pqyis60e0rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1fpd0mv</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Oil soaking improved my natural c-curve</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpd0mv/oil_soaking_improved_my_natural_ccurve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1fpczmv</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Questions from beginner: shellac vs dip powder french mani</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpczmv/questions_from_beginner_shellac_vs_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1fpcvzp</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Nails keep breaking at corners 🥲</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpcvzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1fpcqua</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Cat’s eye ruby red gel mani</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ps5j1h3c90rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1fpcin7</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done for the first time in a year! </t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpcin7</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1fpc3mv</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>I let my BF pick my colors &amp; accent nails</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhr80b1j40rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1fpbrnx</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Soul eater nails</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpbrnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1fpbq6s</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>how can i make my nails look better without polish that covers them?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpbq6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1fpbnzp</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lpbj2m810rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1fpariv</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First Japanese gel Mani (this time with a pic!)</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpariv</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1fpa74l</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>gel damage</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpa74l/gel_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1fp78jz</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>What is wrong w the nail?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dil6879j4zqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1fpa0pe</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Silly question: Can I do chrome with a regular topcoat?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpa0pe/silly_question_can_i_do_chrome_with_a_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1fp9mv3</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple design on natural nails for my daughter </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kbs7l76mzqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1fp9mp0</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Low-key in love with this combination, Part 2: in action.</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rn4jmal4mzqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1fp9d04</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Best way to clean up Cuticle/Proximal fold</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp9d04/best_way_to_clean_up_cuticleproximal_fold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1fp9bjx</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Fall season woohoo!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6hpx03xjzqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1fp983h</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Blue or green?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp983h</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1fp90ap</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>First full set I made!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47hc6kzmhzqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1fp71sa</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Which press on nails do you recommend?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp71sa/which_press_on_nails_do_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1fp6ayf</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Any tips?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp6ayf</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1fp6260</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Lil Peep inspired nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp6260</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1fp5d31</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Dows this color and shape suits my nail shape and skin tone?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp5d31</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1fp8su0</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Princess Nails </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybies5h4gzqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1fp8mna</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Sistaco or Manicurist</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp8mna/sistaco_or_manicurist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1fp8cmx</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Low-key in love with this combination: </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp8cmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1fp8bsk</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Natural  💗 (Sheer pink)</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qdi07t4kczqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1fp8akn</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Asked my tech to do pumpkin spice nails</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnclf1kbczqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1fp7sr3</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bought this color changing press on nails and they look terrible, idk how to fix them </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp7sr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1fp7sg1</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Is drilling required for dip/SNS?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp7sg1/is_drilling_required_for_dipsns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1fp7lkk</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Purple mozaïc pedi</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp7lkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1fp7bti</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>spooky scary skeletons 💀</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krvfl9385zqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1fp7be6</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Im just in luv with these nudies 😌</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xduo65p45zqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1fp74zj</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>My regular polish nail arts! Hope you like them because I really did 💅🏻</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp74zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1fp6niy</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>CLEAN UP ON AISLE 1</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw9pxfka0zqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1fp6in0</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>First time getting Japanese gel (or ANY professional gel!)</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp6in0/first_time_getting_japanese_gel_or_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1fp5qtb</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Im obsessed. </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a97vp69htyqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1fp5ol9</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>32 years old and getting my first manicure- please advise!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp5ol9/32_years_old_and_getting_my_first_manicure_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1fp58u9</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Red nails with white spots and the puppy wanting my attention 🥰😅</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yez8qqmlpyqd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1fp4f6c</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Brand and Lamp advice please</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp4f6c/brand_and_lamp_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1fp4696</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>What kind of glitter is your favorite to use on nails? ✨️ One of mine is reflective 🤩</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a62np4hugyqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1fp4071</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>What do u guys think of these</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp4071</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1fp3omp</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>20 minute gel stars</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqwkb2hpcyqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1fp2wka</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails for a date! </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpcigaku5yqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1fp2ean</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling blue </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp2ean</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1fp2dhs</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Press ons💅🏼✨</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp2dhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1fp2cgv</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>silver cross black coffin XL nails</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nb6zoeuc0yqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1fp1fa5</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BIAB recommendations </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fp1fa5/biab_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1fp18o3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>I usually go for warmer tones but I like this!</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxho0lw0oxqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1fp0ng6</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>fresh nailzz</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irsv7t4xgxqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1fozhq1</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>I literally have no idea what art to do on them</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxdz1kb81xqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1fpov3v</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>BKL - The God and the Gumiho mysteries question.</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpov3v/bkl_the_god_and_the_gumiho_mysteries_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1fporj9</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Im re uploading the pic of my new Icy powder and is the Moyra mirror pigment powder N. 8</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/183jul5083rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1fpkshv</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time nail stamping. I'm really living the results </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpkshv</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1fpobgj</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink goldfish vs baroque </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpobgj/pink_goldfish_vs_baroque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1fpny2k</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Matching the morninglories</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7p7ilhoy2rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1fpmkyc</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Need Some New Brands to Try</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpmkyc/need_some_new_brands_to_try/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1fpm9dl</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Speckles!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eh657mldh2rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1fplgq9</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>ILNP Sunday Brunch or Similar - HELP!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wke2ffqp92rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1fpkp88</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your favorite must have green? </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcvdg2dn22rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1fpko0j</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Sub Updates: Mod Applications &amp; Banner Contest! 🐸</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>/r/RedditLaqueristas/comments/1f6lm5l/sub_updates_mod_applications_banner_contest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1fpkjw0</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>I was going to go dark and moody today, but then I became ✨fabulous✨</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpkjw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1fpkczc</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>First attempt at coloured french tips!</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpkczc</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1fpk4ir</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>ILNP Amazon Black Friday Sale</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpk4ir/ilnp_amazon_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1fpjvmd</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Peel off base</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpjvmd/peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1fpju9m</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Juicy and Glowy</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpju9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1fpjm3n</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Ünt Ready for Takeoff Discontinued?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpjm3n/ünt_ready_for_takeoff_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1fpjgff</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Gradient Stamping</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpjgff</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1fpg24j</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite jelly atm… </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpg24j</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1fpj6of</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">#130 -Soverign </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpj6of</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1fpj5wy</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>One of my students told me it is time for fall nails!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpj5wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1fpiz58</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>What is going on with this Dark and Stormy Clionadh?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpiz58</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1fpitl2</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>"Le Griffon" by LynBDesigns 🍂</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpitl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1fpih25</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Not sure if it works for me😅</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qd7ss0hi1rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1fpievf</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>found a bunch of OPI minis at the dollar tree today!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpievf</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1fpicoq</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>"Well hey there good lookin" - Me, to my nails</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpicoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1fpi9vn</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Something slightly more blue/grey</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpi9vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1fpi2ll</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Access Denied 👽</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpi2ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1fph6a0</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching my car lights! </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoqae0fk71rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1fph084</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Difference in thermal longevity </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fph084</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1fpgyqn</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nails </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9ca3lnr51rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1fpgkxk</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>It’s giving…middle school notes to your friends 🖊️ 🌸 TTYL!</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpgkxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1fpgitc</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>ILNP Skye 🌌</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jog4sk9921rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1fpfgtp</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>First set of polish since i was a kid</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pam4cowt0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1fpex0j</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>🍇 grape nails 🍇</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0lblifqp0rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1fpdt98</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Any photos of nails that grew back?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpdt98/any_photos_of_nails_that_grew_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1fpca3o</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>I think I finally get the "donut glaze"/chrome hype</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpca3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1fpc3ki</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love magnetics </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oqeyolli40rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1fpc1ta</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Feeling Still Mixed on the ORLY Terrazzo Topper</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpc1ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1fpbznb</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Why is it near impossible to get a good picture of Pearl Jammin’ 😭🥲</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpbznb</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1fpbzdj</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help finding proper magnet </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ju5tpfn30rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1fpb84l</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions on Cirque Colors thermals + Wedding Nails? </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bmiu0j5xzqd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1fpb2y8</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Super Duper Juiced</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpb2y8</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1fpausa</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Matte black 🖤 giving 2015 in the best way</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpausa</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1fpa99v</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Should my gf push her cuticles back?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpa99v</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1fp8ymo</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>There Are No Prizes in the Game of Hearts</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp8ymo</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1fp8f2i</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Finally kicked my nail biting habit!! Now I'd like to build a polish collection from scratch, and would love your two cents. Help?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yax3cn9dzqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1fp7wvb</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Clionadh Nucleus Accumbens</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d3rnsqk9zqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1fp7s8q</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Accidentally matched my onion</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp7s8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1fp6dvh</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Too much thinner in top coat?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fp6dvh/too_much_thinner_in_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1fp5rve</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>ILNP Chai Latte</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp5rve</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1fp5lwu</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Great fall creme, mediocre formula. </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp5lwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1fp50t1</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you paint your nails, and then start seeing that color EVERYWHERE </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp50t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1fp4or2</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Feeling wine-y 🍷</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp4or2</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1fp40oz</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>How does ordering from Bee’s Knees work?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fp40oz/how_does_ordering_from_bees_knees_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1fp3jsv</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This one is crazy gorgeous for fall! </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp3jsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1fp3imp</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Chrome powder for regular polish?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fp3imp/chrome_powder_for_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1fp30ma</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your favorite fast-drying, high-shine, long lasting toppers lately? Or in other words, I'm done with Seche Vite. Is there an alternative? </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fp30ma/what_are_your_favorite_fastdrying_highshine_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1fp2xws</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Does hand sanitiser affect your manicure?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fp2xws/does_hand_sanitiser_affect_your_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1fp2jav</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>After all yalls manis 😈</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oizpjuib2yqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1fozk99</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Tiny nail bed Brushes?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fozk99/tiny_nail_bed_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1fpqy97</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Love me some scribbles</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9d8jjet04rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1fplvjw</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>💜💜💜</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gh5t3cpmd2rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1fplafe</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Second attempt at last nights nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fplafe</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1fpl45u</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did Halloween nails on my bestie! </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iualbpvi62rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1fpkp7r</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Still learning but definitely making improvement. Here’s the last set I did on myself</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08pb6c8n22rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1fpion1</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Was feeling some white fall nails.</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjzex9vak1rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1fph15e</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyy5ip2e61rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1fpfmfj</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>concert nails❤️</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpfmfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1fpew77</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Nails for my wedding this weekend 🤍</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpew77</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1fpdqtj</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another attempt </t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpdqtj</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1fpdd9s</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail foils! Went well♥ </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyb4pakzd0rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1fpd8nn</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Doodles! IB: @__myohae__ on IG</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpd8nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1fp7nd1</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Purple mozaïc pedi</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp7nd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1fp4yzu</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspiration </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fp4yzu/inspiration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1fp27jc</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fp27jc/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1fp1u05</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do the flowers ruin it? </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt8ggdbquxqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1fp01y6</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Newbie so please be kind</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fp01y6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Sep 27 08:10:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_29.xlsx
+++ b/data/collected_data/2024_09_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C845"/>
+  <dimension ref="A1:C1022"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14798,6 +14798,3015 @@
         </is>
       </c>
     </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1fqi05i</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>first set in 4 years</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuesqlmxxard1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1fqhspb</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Where to find this color in REGULAR polish?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqhspb/where_to_find_this_color_in_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1fqhdk5</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>chat, what do you think? 👀</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqhdk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1fqgzjh</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Obsessed with this color!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko04aurjkard1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1fqf0by</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails(for the first time in a year 😬) what do we think 😍 </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyc3zrwpx9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1fqexc1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>How much would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qywk761vw9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1fqenos</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">baby pink nails 🎀🍓 </t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/959hcfn3u9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1fqef9t</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Does brand of gel polish increase likelihood of contact dermatitis or is it just user error?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqef9t/does_brand_of_gel_polish_increase_likelihood_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1fqel84</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Very cutesy, very demure 🩵🤍</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nkwt92et9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1fqekqc</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Y'all ignore the messy polish. Thinking of getting long coffins instead?? These are feeling too short now...</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ot1sqwg8t9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1fqekgh</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Question: Is base coat for gel polish the same as foundation base gel for builder/poly gel?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqekgh/question_is_base_coat_for_gel_polish_the_same_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1fqeiq9</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Did someone say extra?? I am so in love with this stiletto set😊✨</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqeiq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1fqc7z5</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Tried 3D blobs and flowers for the first time</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqc7z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1fqd8uf</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goal: To grow my natural nails long and strong! Any recommendations for a clear coat that won’t damage my nails? </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqd8uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1fqdyvf</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Structured gel caused two of my nails to break on the nail bed and two other of my nails to break fairly short. I don’t know what to do?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqdyvf/structured_gel_caused_two_of_my_nails_to_break_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1fqdkee</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time making my own set! </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuxnlggej9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1fqd77m</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>What a beauty</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lal0keouf9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1fqd282</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>they were more beautiful 😍</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rfbwovge9rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1fqd1cu</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>bawling my eyes out because the nails I got done for Homecoming TODAY are already breaking. Figured I'd at least post them here for some appreciation :(</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5rwlbe6e9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1fqcmv8</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>What can I do to fix these?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqcmv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1fqcf69</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Don't know how I feel about these</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqcf69</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1fqcah9</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried 3D blobs and flowers for the first time </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqcah9</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1fqc8lf</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I love this pressie set from Kiss so much 🤩</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zszxdjo69rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1fqc592</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Welcome Fall Y’all!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqc592</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1fqc3q9</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at detailed characters like this </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqc3q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1fqbv7z</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>My birthday nails 😘💕🩷</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqbv7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1fqbgny</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>If anyone tells you 3D sculpting on short nails is easy, they are a liar and possibly a witch.</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o08r1vagz8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1fqbfra</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Can you tell these are press ons?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2ojl8v7z8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1fqbf0k</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>simple but cute</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqbf0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1fqbac7</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Latest set🖤🧡🤍</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2o12tx6sx8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1fqanv9</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>proud of myself ✨ cherry cola gel</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqanv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1fqaj82</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I admire my neatness, what do you think? OPI brown with small glitters</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2l28qn6zq8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1fqaez3</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Spinnnerrsss</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mh5m8ehxp8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1fqaeku</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Nude base + glitter + chrome deco✨️</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqaeku</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1fqa8qq</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set that I’ve done </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68qb0ipco8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1fqa5z8</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>somehow, all of my nail polish fit perfectly into the container</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1efxkamon8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1fqa23o</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Kiss X-Tend! $22 for the starter set</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8n1hwdrm8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1fq9uw2</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Why is it spotty?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b30evca0l8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1fq9a9k</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>There’s just something about a good red polish🌹</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq9a9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1fq8yfa</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">YOGO Milk Jam 3D staying soft after curing </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uize5qrfd8rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1fq8sfr</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>perfect red</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w94fsjz2c8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1fq8ms2</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Lincoln park after dark 🥀</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2yemhtra8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1fq8ibv</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Self taught acrylics 💜</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hylm1mr98rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1fq8a10</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Growing natural nails</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fq8a10/growing_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1fq7mt5</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>First time using gel-x and builder gel</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq7mt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1fq7af6</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Super proud of my first real attempt at designs!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq7af6</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1fq77h8</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Tips for my tips?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq77h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1fq3hh0</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why are my nail extensions turning brown? </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fq3hh0/why_are_my_nail_extensions_turning_brown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1fq4cgy</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Inspo pics!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq4cgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1fq6ty1</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>This is my new work. What do you think about men’s manicure with gel polish? 😼</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r36caaaow7rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1fq6mv1</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>i’m obsessed i fear…!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq6mv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1fq6if1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set in 20ish years, so happy </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq6if1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1fq6d2p</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The tape is making me angry. </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/101pt914t7rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1fq6c1h</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>My natural nails with a matte paint on top.</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx5k3gxvs7rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1fq64hr</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>First time at-home mani 🎀✨🫧</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnkg30z9r7rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1fq5lxw</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Ready for Hawai’i</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr60tobdn7rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1fq540v</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq540v</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1fq50pf</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>nail shape &amp; filing?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq50pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1fq4soi</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Since y'all suggested to go for warm tones... instead of nude.</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3u3urj03h7rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1fq48oh</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Pretty Plum</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq48oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1fq3vv5</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Cute fall mani on natural nails! 🍄🍁🌿</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq3vv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1fq3o92</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Commemorating my Childhood :)</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhlz5h1r87rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1fq3g9a</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Nail biter help</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fq3g9a/nail_biter_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1fq28tn</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Dip powder with chrome ✨</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccgnbgz0y6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1fq24yz</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Is there a way to make press on nails last longer?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofldzge9x6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1fq240s</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Latest Set </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6zppc03x6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1fq1us8</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Vacation nails by me! 🌴</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq1us8</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1fpy0gt</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>What do you use to apply your DIY press ons?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpy0gt/what_do_you_use_to_apply_your_diy_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1fpzz2s</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last few sets; acrylic overlay </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpzz2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1fpzwfj</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>plz help me find these polishes</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnr5nj0lg6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1fpwwcc</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>nail polish reacting with gel top coat?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b47k105xt5rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1fpv5q7</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Advice on art brushes etc</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpv5q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1fprgry</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for October nail inspo!!  </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fprgry/looking_for_october_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1fq14wn</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Airbrushed Ombré fall acrylics🎃</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n7eatowp6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1fq14tp</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried butterfly wing </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf0mfeevp6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1fq1196</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short nails </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq1196</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1fq0ycw</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>What can i do to grow my nails longer?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq0ycw</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1fq0r83</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Matching with my shirt Lol</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgv8gxy0n6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1fq0p65</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Help with frenchies!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fq0p65/help_with_frenchies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1fq0ole</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Cadillaquer- Saffron (reflective)</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq0ole</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1fq0l8l</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Pretty pink nails 💕</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m1vl0patl6rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1fq00hq</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Me gusta lo diferente 🖤🤍 que les parece chicas 🤗 divino no</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0xmibvdh6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1fq004w</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last few nail designs </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq004w</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1fpzhcl</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back with a fresh ballerina set 🩰 </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nc8tca7id6rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1fpzehs</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went Burgundy for fall </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpzehs</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1fpzeg6</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>found my favorite shade of white :)</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpzeg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1fpysj8</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>I love wearing the pedicure and the matching manicure 💅🏽cherry 🍒 Who else likes to wear the matching nail polish?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gywlmuyd86rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1fpyp5r</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>My Halloween Nails!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ei7zero76rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1fpyhkv</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gels nails don’t last </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpyhkv/gels_nails_dont_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1fpxqs5</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Camouflage base coat 🎀🩷</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cxpa3vh06rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1fpxjin</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My sister-in-laws first set of custom nails 👻 </t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpxjin</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1fpxi5y</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love French nails </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7kblm8my5rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1fpxbhk</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my nail tech did her thing </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpxbhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1fpxa6j</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went to nail tech student as a hand model, what do u think about them? They’re acrylic </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gbkesfvw5rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1fpwzyb</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tentei achar uma foto só da unha mas não tenho uma tão boa :/ porém essa unha ficou tão linda quando fiz que precisava compartilhar aqui!! </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpwzyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1fpw6q0</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Super Glue 😬</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpw6q0/super_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1fpvtmx</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Tiny dot indent on nails?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0t5ntd0l5rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1fpu5d0</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>nails growing upwards at the tip</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fpu5d0/nails_growing_upwards_at_the_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1fptsml</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All set for spooky season </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fptsml</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1fprg5b</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Loving the simple look, but what fun shape or color could I try next?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fe87w1yt74rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1fqiqnv</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Sabertooth on a mountaintop</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqiqnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1fqhm0g</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>ILNP jinx for spooky season</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqhm0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1fqhjfm</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>dupe suggestions for  Blossom’s Firebreath</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqhjfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1fqgoh5</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Shockwave and anatomy study </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scuut09mgard1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1fqe7fn</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Fancy Gloss restock question</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqe7fn/fancy_gloss_restock_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1fqe38i</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Favorite iridescent magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxe7htgio9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1fqdrww</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>PPU late to ship?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqdrww/ppu_late_to_ship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1fq2twd</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>DVN quiet dreams</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq2twd</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1fqddim</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Seche Blur Experience???</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqddim/seche_blur_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1fqdcci</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bill has to be the shiftiest polish I’ve ever owned. </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xdjjj1c6h9rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1fqd307</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stained Nails - Polish Recommendations </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqd307/stained_nails_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1fqd23w</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Astromancy Mani and Axolotl Mini</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5el1keie9rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1fqcz82</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Significance/important of not flooding cuticles?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqcz82/significanceimportant_of_not_flooding_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1fqcied</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oh My Gourd </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqcied</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1fqc9jb</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fav Halloween colors/combos? 💜💚🧡(pic of Venus Flytrap for attention) </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chbm7ozw69rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1fqbusi</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Hurricane ready</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/neg9u79539rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1fqbeg8</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enchanted - Cirque Colors </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ro7hbbuy8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1fqb20l</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Magnetic depth</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqb20l</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1fqav2d</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>This combo is so pretty</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqav2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1fqa9yr</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Be honest, how is this color on me?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqa9yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1fq9uz2</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Something spooky is brewing… 🔮</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq3dal</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1fq9s0q</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why has it taken me this long to try a Reflective polish?! Oh my god! </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pnrv182bk8rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1fq9do3</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Essie’s Bubbles Only is my new love 🌹❤️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq9do3</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1fq86v9</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Addiction turning to hobby!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq86v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1fq847e</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>What is it in Essie's cuticle oil that smells so good?!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c53ptv9l68rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1fq80tb</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">k l i m t 🥲 </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfasbyev58rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1fq7cnr</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Seeking an ideally affordable OPI “Aloha” dupe please</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lgxm5hn08rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1fq6dfp</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Simply Faaake</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lmlkwq55t7rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1fq61bu</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>All ya’ll’s fault! 😊</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k06cxhbmq7rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1fq4l6r</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>I understand the LynB hype now 😩✨</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq4l6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1fq4ka4</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merkitten realness </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq4ka4</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1fq3pso</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Not my best work, but I still enjoy :) my almonds are growing so fast! Nit sure I love how much upkeep they are 🥲</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq3pso</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1fq3ayk</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Aspen by ILNP is stunning 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq3ayk</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1fq2mwn</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting started with decals </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq2mwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1fq1qfy</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Versatile chrome topper ✨✨</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq1qfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1fq1jtx</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Sale question</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fq1jtx/sale_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1fq1haj</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>✨ Prism Parade's Alchemy Collection [Paid PR]</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq1haj</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1fq1ecz</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Re-donk-ulous shrinkage!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq1ecz</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1fq1c93</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>fall pruglie and new cursed poses to go with it</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq1c93</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1fq13vh</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Can you recommend a better neutral-ish pink for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq13vh</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1fq0pa8</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Cadillaquer - Saffron (reflective)</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq0pa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1fq0ldg</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you guys post polish photos without this weird solar flair effect? </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs9o2jhul6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1fq065j</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Will Nailtiques Formula 2 work over a base coat?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fq065j/will_nailtiques_formula_2_work_over_a_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1fq05th</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Which brand’s toppers do you like best?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fq05th/which_brands_toppers_do_you_like_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1fpzx5a</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Kitty Nails!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05voejsqg6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1fpzb21</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Late Checkout is super beautiful </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpzb21</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1fpywy4</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>ISO a polish to match them!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpywy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1fpy4nk</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Dark Academia Nails</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xg6sdpg36rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1fpy4dn</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Hispanic Heritage month</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpy4dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1fpwym3</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>That purple shift 😍</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpwym3</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1fpwolk</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>First manicure in years</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hpmpng6s5rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1fpwagi</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Mooncat vs. Cirque comparison</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpwagi/mooncat_vs_cirque_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1fpw1t7</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Opal vibes for fall 🍂</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd2jfwivm5rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1fpvwtp</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Mooncat Drop</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpvwtp/mooncat_drop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1fpvkzm</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Can I use a different brand base coat and top coat with death valley nail polish?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fpvkzm/can_i_use_a_different_brand_base_coat_and_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1fpul5h</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>dark horse by mooncat</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urt2wxjs95rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1fpt8mg</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>ILNP Evermore - First time doing Lacquer after gel use and wowwww</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpt8mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1fps2bj</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>This might be my new favorite combination:</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fps2bj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1fqebi3</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Feeling Coquette</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/djoyoujqq9rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1fqd20g</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>So I tried doing my first ever tiktok. Not only did I fail that but this is not Mt favorite design. It need some work. BUT I'm proud of myself for putting it out there!</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ly6yh7ae9rd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1fqc2z3</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Halloween Nails from last year!!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqc2z3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1fq9de7</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>My first proper attempt at something cohesive</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkeobjavg8rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1fq8amg</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Blue and glitter ✨</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpweglt188rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1fq64qo</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Eco friendly sequins</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fq64qo/eco_friendly_sequins/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1fq5yr4</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Halloween 🎃 fun</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq5yr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1fq4eq1</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Diseñó 💕</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akq28629e7rd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1fq463o</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I need inspiration. Lately I've been in a state of zero mood and inspiration. I love to make caricatures and landscapes, I share with you two of my practices. </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fq463o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1fq3x6i</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Love it or not</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1payaqgma7rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1fq29ku</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>I have so much respect for nail techs. How y’all do this in 1.5-2 hours a client is beyond me. This is my first attempt at nail art, second attempt at gel x application. Went for a retro 70s vibe.</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8p3cls5y6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1fq24l0</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Eeyore Stitch, tigger Stitch❤️</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rigymay6x6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1fq1u32</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Is there a subreddit that does nail art challenges? Or does this subreddit have one?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fq1u32/is_there_a_subreddit_that_does_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1fq1g57</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Nails🤩</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbgzv1e8s6rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1fpyff9</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>☁️ new nails</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fpyff9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1fpvqeu</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second hand </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6xy4l18k5rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1fpu3v1</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>beginner nail tech work</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8r14zb155rd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1fptpk4</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Spooky season nails</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fptpk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1fps74l</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love pink and glitter. What about you? </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4aao2sz8i4rd1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Sep 28 08:09:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_29.xlsx
+++ b/data/collected_data/2024_09_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1022"/>
+  <dimension ref="A1:C1197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17807,6 +17807,2981 @@
         </is>
       </c>
     </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1fr9as1</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Have you tried Holo Taco?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fr9as1/have_you_tried_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1fr90ko</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haloween set! (Tips and constructive criticism are welcome!)🤗 </t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr90ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1fr7s35</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr7s35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1fr7ruj</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just saw on eBay a new 2024 Nailtiques 2 </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fr7ruj/i_just_saw_on_ebay_a_new_2024_nailtiques_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1fr7k78</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New here, looking for advice. </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fr7k78/new_here_looking_for_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1fr70gj</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>My Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8yhdgfnghrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1fr6xkx</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Subtle</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljlyt41ofhrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1fr6c4r</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wanted to do something nautical themed for my cruise </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9e8hhvp8hrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1fr5s9p</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Plain is attractive</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gho1pohj2hrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1fr47gn</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Theyre not great but I'm slowly getting better at gel nails! Used Madam glam gels </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr47gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1fr46v2</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Black on black🖤</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fiszpujplgrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1fr453s</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>BLACKPINK BLACKPINK🎶</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr13act7lgrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1fr43nb</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My new favorite top coat!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr43nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1fr42ol</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love these little flowers 🌸 </t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spgrqrgjkgrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1fr40fo</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Got the courage 😂</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvt2c7qwjgrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1fr3sr6</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Demon Slayer</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruyaynhrhgrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1fr3shf</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>🌟💚</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hliup6qohgrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1fr3pdx</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>what do you think? It's something simple</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cms6aisggrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1fr3k6g</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>3D Flower Acrylic Nails</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scos26i4fgrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1fr3ird</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Pistachio squiggles 💚</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00nt8rfxegrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1fr343w</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Green marbled Snakeskin</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/simyoxzuagrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1fr2wzi</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>What do you think? Does the middle nail with the heart look good with the design or is it too much?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44v910iy8grd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1fr2wb6</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my nails match my knife 💅 </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8kwvvrr8grd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1fr2sao</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Guess who discovered nail stickers :)</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr2sao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1fr25yt</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Unintentional but ended up with a holiday vibe</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5a5xlep1grd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1fr24ql</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Loving my woodsy nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fr24ql/loving_my_woodsy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1fr20oc</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>supa long naillsss</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr20oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1fr1v9s</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fr1v9s/recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1fr0shw</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>First Nail Design vs Now</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr0shw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1fr0s0r</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr0s0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1fr1ioa</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is one week too soon to replace my nails? </t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fr1ioa/is_one_week_too_soon_to_replace_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1fr1amc</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ex biter </t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaw9tgwrtfrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1fr16hw</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love basic nails </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85icpsqrsfrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1fr0wk9</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Ohora nails</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km0phgabqfrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1fr0hth</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Magnetic heart !!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zi4gh5hqmfrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1fqztu7</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Fun Halloween Nails 3D</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqztu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1fqz1xs</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Look it FREAKING BATS 🦇 </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1kie287afrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1fqz1xq</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Am I crazy and too picky?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pg5466v7afrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1fqyyuh</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Halloween nails! 💀 </t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfkfstci9frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1fqypiu</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Drew my inspo and brought it to the salon, they turned out cute 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqypiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1fqy620</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">bloody halloween set </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqy620</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1fqylf5</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall but sparkly ✨ </t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k72gyocf6frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1fqyfo7</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">where can i find these nail tips online or on amazon? </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdl06jj35frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1fqyc03</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made myself press ons for Oceans calling! </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqyc03</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1fqy67g</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what color is this? </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6buj99y2frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1fqy266</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My ombré witchy nails riding the 7 train in Queens, NYC. </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnb24vu02frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1fqxuql</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Latest set</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzyqpx0d0frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1fqxp2c</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone tried using Gunpla decals for nails before. </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqxp2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1fqulka</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Question/Advice: Gel-like Top Coat Replacement Recommendation</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqulka/questionadvice_gellike_top_coat_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1fqw41r</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Inspired by my Tamagotchi 🩷</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kezvk4mmerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1fqwyz0</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my tech so much!! </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqwyz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1fquy6i</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first attempt at character art! over the garden wall inspired set </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fquy6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1fqxehe</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Tried something new today</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c66v3onwerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1fqx55v</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>120$ nails</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5555uqouerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1fqx16o</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Long Rectangular Nails?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqx16o/long_rectangular_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1fqwzag</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>How do these people get certificates?!?!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvhtjtueterd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1fqwxee</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started to do my own nails at home </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqwxee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1fqwtht</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>salon etiquette question...?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqwtht/salon_etiquette_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1fqwshq</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite nails </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/080m6c6yrerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1fqwk2z</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Decided to wait to do fall nails. 🐆🐅💅🏼</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nbryxu5qerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1fqw9ug</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Essie 'Wicked'</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3qzdzfwnerd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1fqvtx8</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Which nail polish protectors to use?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqvtx8/which_nail_polish_protectors_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1fqvsj0</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>First time doing brown, what do we think?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqvsj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1fqvmn9</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Autumn nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wfgkt0tierd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1fqvkkk</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>What are your thoughts about my nails? 😌</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqvkkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1fqv0dm</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Simple Pink Nude</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sga1akjwderd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1fquvtj</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Simple nails!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1zn8f5xcerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1fquu4l</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Nail color suggestion for pink dress + rose gold jewelry</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0gtluqbcerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1fqus94</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matched my nails to the sunset </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqus94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1fquh45</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fquh45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1fqucn0</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips for growing out nails?? </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqucn0/any_tips_for_growing_out_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1fqtv6m</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>🍂🍁 ILNP Fall Serenade Bundle with Holo Taco Fallen Flake Taco as a topper 🧡🤎</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqtv6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1fqtgpz</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail dump 🫡 (first mani inspo from @kiracyan.designs (IG) via CASETiFY, second mani inspo @agathesinger on IG, third mani inspo @damonxart on IG) the rest are freestyles </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqtgpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1fqt6ts</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i did some gel x on myself! any advice welcome </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqt6ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1fqt4ia</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bday Nails </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbum9s6azdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1fqt3dd</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic for October! ( a few days early) </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c99oigt0zdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1fqspyk</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sugar cookie nails </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zejud35wdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1fqsobf</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>New set 😍😍</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6maa56svdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1fqsidw</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>elegant and at the same time modern💅🏻</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgqh2pkkudrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1fqsfvj</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Did someone say beetlejuice?💚</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqsfvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1fqrknn</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>What do I choose? Lol, booking online and I’m so confused!!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/li6hbg26ndrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1fqs9o7</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail removal? </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqs9o7/nail_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1fqsbjp</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first acrylic set </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btqlyn32tdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1fqs7b8</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dazzle Dry nail art anyone? </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqs7b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1fqs1qi</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Happy with short nails!!!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wl4tu7xqdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1fqrj42</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Advice please!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqrj42/advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1fqmw76</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seeking suggestions </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd4ii8dqlcrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1fqkxcj</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>How to get chrome to let the color underneath show</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqkxcj/how_to_get_chrome_to_let_the_color_underneath_show/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1fqmvfg</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Semi cured nail strips</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqmvfg/semi_cured_nail_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1fqpk09</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Nail art ideas :)</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqpk09/nail_art_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1fqrwxa</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My birthday nails </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izlwdn5vpdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1fqq8sx</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I want to do other people's nails but it takes me forever</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fqq8sx/i_want_to_do_other_peoples_nails_but_it_takes_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1fqqwke</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>UV Gel nail stained</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1qla4s5idrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1fqrg61</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shocked this 5 day old mani survived post-Helene cleanup! </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g4mw328mdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1fqrhow</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Fall has arrived! 🤎🍁</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqrhow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1fqr9j7</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Anyone else weird like me</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqaq5iotkdrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1fqr34g</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Forest Fairy Vibes</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqr34g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1fqqtbb</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Spooky but make it professional</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqqtbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1fqqj31</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>I'm super in love with these for some reason</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqqj31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1fqqg78</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Question never got my nails done lol</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s5cbqnpedrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1fr8mpb</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Uneven nailpolish from big flakes?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fr8mpb/uneven_nailpolish_from_big_flakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1fr7sms</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Reminiscing 😔</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9f545d1bqhrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1fql3mj</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Seeking advice for ridged nails</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fql3mj/seeking_advice_for_ridged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1fqmb86</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP candlelight </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqmb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1fqvl86</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Electric Summer + Black = Spooky Season?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqvl86/electric_summer_black_spooky_season/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1fqu239</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Polish thinner?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqu239/polish_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1fr4sww</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>🐸</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzh1oxcyrgrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1fr4gcx</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6.5 weeks without chewing my nails - usually only change once a week but my nails just felt like they needed love again.  </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv580phbogrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1fr4fxz</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>green apple jolly rancher</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr4fxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1fr46jx</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Has anyone heard this?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mcisk3ahkgrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1fr3xy6</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NP haul from Ulta! Thankfully delivered in good condition </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr3xy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1fr3ijt</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pleasantly surprised with this nail polish! </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr3ijt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1fr2pnl</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>My first time water marbling</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>/r/simplynailogical/comments/1fr2p0a/my_first_time_water_marbling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1fr2ovn</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Just received my Holo Taco order from Ulta 😞</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp0znxsr6grd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1fr2j77</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Mooncat thermal Treachery in blue</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr2j77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1fr2dhy</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Minimalist natural nail with flake</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv04xaao3grd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1fr2aqz</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Fancy gloss shop opened today</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fr2aqz/fancy_gloss_shop_opened_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1fr2aax</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>and that's on a LONG day at work</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr2aax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1fr28va</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>OPI Wicked spotted at CVS</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr28va</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1fr1y2c</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My descent into madness begins </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkkliq3ozfrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1fr1qdr</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Swatch Request: Mooncat Memento Mori and Orly Ephemeral</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fr1qdr/swatch_request_mooncat_memento_mori_and_orly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1fr1ndg</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Dollar Tree Canada polish love</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr1ndg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1fr0rhl</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>I told myself I would only order 2 thermals per year 🤡</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcihng43pfrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1fr0mle</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>I had so much fun painting blobs and lines</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr0mle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1fr0a0k</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vampy? </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rshlzvrkfrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1fqzd98</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Scored too big, if that’s even possible</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqzd98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1fqz6k6</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Combo of my Barbie dreams :’)</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqz6k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1fqyj0k</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>SWATCH REQUEST - By Dany Vianna: Hot Toddy, You Furry Thief, Color Bomb</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fqyj0k/swatch_request_by_dany_vianna_hot_toddy_you_furry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1fqyb23</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Looking for something similar to Cirque’s Rose Jelly from OPI or Essie</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.cirquecolors.com/products/rose-jelly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1fqy9e2</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Got very distracted by my nails on the way home from work 💅</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqy9e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1fqy8oa</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love yellow/greens </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqy8oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1fqxyh6</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>I found a shirt that matched my shifty nail polish~</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1u9xr0081frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1fqxkc3</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Rainy days is gorgeous 🌧🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu15pwc0yerd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1fqwu8u</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Someone here told me about the Cirque Jarritos line and all I wanna say is THANK YOU!!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6h3xcl9serd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1fqwbd8</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>🧲 30 lb horseshoe magnet changed my brain chemistry</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqwbd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1fqvtx6</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this floral look! </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7178hickerd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1fquxiv</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Violet Riot - Sinful Colors </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo9ooigaderd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1fqus1d</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Choose Life (magnetic) - bee’s knees</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqus1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1fquc0i</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Candlelight 🕯️</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5hxxwrci8erd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1fqtz65</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Fell in love with nail polish again</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqtz65</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1fqtubr</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>🍂🍁 ILNP Fall Serenade Bundle with Holo Taco Fallen Flake Taco as a topper 🧡🤎</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqtubr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1fqtt14</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>More thermals!! 💜</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s467zzwi4erd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1fqtinc</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>If I ever become a vampire, I will only wear this color.</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqtinc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1fqswmf</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>It's only going to be 107°today, very Halloweenie 🎃💚</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqswmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1fqsgmu</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>EDM - Half Orange</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/afithu54udrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1fqrp86</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>“Intensely Shifty” indeed</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqrp86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1fqpp5v</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freshen up your mani for the weekend with a sparkly topper </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqpp5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1fqpkvr</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UPDATE! It turns out dishwashers reverse the effects of a washer and dryer on polish! Or J&amp;B was sweet enough to replace my bottle, both options make sense to me. </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv3edgny7drd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1fqoy2z</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Today was a good mail day</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjdhldbz2drd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1fqonud</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Favorite season has arrived 🍁</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1s7zjqp0drd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1fqonl4</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>had a suggen urge for plain red ❤️</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clg77btn0drd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1fqoddi</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>First time doing nail art: proud and want to show off!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqoddi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1fqobtk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Chartreuse</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/26-9-2024-JHOTYIZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1fqn040</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>are my nails overfiled? advice needed</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqn040</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1fqjq3x</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>3 year old daughter did my nails</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyo9t5ptlbrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1fqjalu</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Purples</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqjalu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1fr90lz</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Soot-Sprite Ghibli Nails</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr90lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1fr7qfc</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky 👻 Fall 🍁 Nails </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr7qfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1fr7bf9</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I loved this design I made</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd6i5f6dkhrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1fr30do</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3il014nv9grd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1fr1aoh</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>New set 🍁</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw4rf26rtfrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1fr19ht</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sanrio nail art by Amy from true touch nails </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tb8m9u4htfrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1fqy6qr</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here’s my nails I matched to my cup </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqy6qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1fqy57v</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling extra special today </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jhjp31q2frd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1fqugip</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails 🎂 </t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqugip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1fquc18</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>cowboy inspired</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fquc18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1fqu4oe</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Lacey - Probably my favorite at so far</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqu4oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1fqu1jk</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Newbie having fun</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqu1jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1fqtq4y</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Halloween girly vibes 😏✨️🧸</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqtq4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1fqosp6</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best pen to make thin design lines or just french manicure? </t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fqosp6/best_pen_to_make_thin_design_lines_or_just_french/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1fqmt5h</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just a little trial 🌹 </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n24zs2kykcrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1fqmprs</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Sweetie pie nails</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqmprs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1fqmngj</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Drag Race inspired 👑</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fqmngj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1fqmbys</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Fall Set </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i73xxeifgcrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1fql1bj</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These need some oomph and I don’t know what </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ntxnkco2crd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Sep 29 08:10:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_09_29.xlsx
+++ b/data/collected_data/2024_09_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1197"/>
+  <dimension ref="A1:C1377"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20782,6 +20782,3066 @@
         </is>
       </c>
     </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1frz7wk</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Stick on nails</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frz7wk/stick_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1froiur</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are they as bad as I think? </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1froiur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1frwls0</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">does anyone know how to get makeup stains off of acrylic nails? </t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frwls0/does_anyone_know_how_to_get_makeup_stains_off_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1fry39h</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Is it bad to not tip a nail salon owner?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fry39h/is_it_bad_to_not_tip_a_nail_salon_owner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1fry14u</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>cute lil combo 💗</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0eonqvqyord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1frxj15</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do my nails grow too fast for this?! </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx94mdjisord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1frx3w3</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian manicure obsession! </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2uds5abnord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1frwo0u</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>First autumn nails ✨</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frwo0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1frv5zc</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Loving these chrome nails 💖✨️</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frv5zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1frv4m2</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>celestial stars and gold crescent moons✨💫🌙✨</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lt62aw51ord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1frukz1</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Fiberglass nails: heeeeeeelp</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frukz1/fiberglass_nails_heeeeeeelp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1frue5v</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>3D hanging cat nails for Halloween 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frue5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1frsie0</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Handheld UV light for curing Japanese gel?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frsie0/handheld_uv_light_for_curing_japanese_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1frt28m</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wife's nail techs hand drawn art. </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frt28m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1fru1r6</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer - Fun With Foliage 🍁</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fru1r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1fru1ex</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>My first "go" at short almond.. can I get yalls opinion?</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fru1ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1frspdq</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Got these done a few weeks ago and i already don’t wanna get new ones they’re so cute!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqxeonzocnrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1frsit8</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>After bath nails 😅</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frsit8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1frsgvr</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Xenomorph nails</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frsgvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1frq0xr</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">halloween set 💚🎃 </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frq0xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1frrt1o</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Entomology-inspired set for pre-spooky season</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frrt1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1frnben</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>First attempt at Gel-X</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frnben</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1frm20d</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Can you do aura nails with regular polish?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frm20d/can_you_do_aura_nails_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1frs8hk</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diosa brand press on nails for the tail end of September - i love the chrome effect </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frs8hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1frs1jd</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel extension kit for a gift </t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frs1jd/gel_extension_kit_for_a_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1frrrm1</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Throwback to Valentines 💘 </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4f7krzk3nrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1frrlqi</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help!!! </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frrlqi/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1frr3py</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Proud of my natural claws </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzo2j8dhxmrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1frr372</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>i’ve had my gel x on for a month, can i just do a fill?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frr372/ive_had_my_gel_x_on_for_a_month_can_i_just_do_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1frqy38</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Ombre nails! I'm in love!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frqy38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1frqwo9</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Nails for Japan!</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frqwo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1frqiop</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>My nail lady killed it with these dessert nails 🥞🍞🫐</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frqiop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1frqbmh</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Re did my mushroom glow in the dark nails, to see decals better in the dark, the first colored background didn’t show them good like this, definitely shopping for more glow in the dark colors and cool decals for spooky season!👽💅🏾🔥🌈✨☄️⚡️🌻💖😍🥰😁</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frqbmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1frpqnj</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI - millennium mocha </t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1rljh1almrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1frpq52</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just got dip nails done for my first time and hate it </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frpq52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1frpous</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Missing toenail-no nail bed</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frpous/missing_toenailno_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1frpekx</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these press ons </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frpekx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1frp93t</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails featuring baby bump! </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nguce1kxgmrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1frp527</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Soooo does super glue actually work?</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frp527/soooo_does_super_glue_actually_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1fro8y7</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Black and white floral set</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fro8y7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1fro8bz</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this normal for gel nails? </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fro8bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1fro7nl</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Natural nail routine?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fro7nl/natural_nail_routine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1fro67e</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Does super glue actually work?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fro67e/does_super_glue_actually_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1fro5eh</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Something simple ;)</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkit83x67mrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1frnooz</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Pink Spooky Nails</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frnooz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1frno81</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>French manicure with dip powder</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhhoe0b93mrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1frnjqn</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regular nail polish </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frnjqn/regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1frnfq5</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Gel X or Natural Nails? It takes me forever to shape my own nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm4axnka1mrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1frneuy</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Completed my first nail course today</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frneuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1frn54m</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Less nonsense </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frn54m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1frn2ke</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Stevie Nicks nails!</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frn2ke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1frn2ho</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>been doing my own gel x!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq7bexk7ylrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1frmo4i</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>My recent work 🥰</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4kw3xzyulrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1frmnx3</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Cute little mani while I’m home recovering!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frmnx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1frmbkg</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude sparkle nails, do you like it? </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiye14g3slrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1frlhij</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>new set done @ home!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frlhij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1frluz8</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>lil ghosties 👻</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kouw9vc8olrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1frluk9</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Acrylic Fill Question</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frluk9/acrylic_fill_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1freu35</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to do with cracked gel polish? </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tq9p32t2krd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1friukx</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>What did she use on my nails?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1friukx/what_did_she_use_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1frlrak</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Perfect shade of purple 💜</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frlrak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1frloiq</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New press on nail set </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frloiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1frfva1</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>My sakura blossom inspired nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cj51fqosbkrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1frlmo8</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail color would look best for fall wedding with burnt orange color dress and nude shoes ? I was thinking nude nail but I wasn’t sure with the nude shoes </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frlmo8/what_nail_color_would_look_best_for_fall_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1frlk4w</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Normal for 2 days after?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugc87sitllrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1frksnq</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Been a while 💚💚</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf3z726oflrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1frkrsm</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>I’m officially a mermaid now 🧜‍♀️✨🦀</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5v4bb2hflrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1frkgdg</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>How can I be quicker? (These took me FIVE HOURS)</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2ugo1jvclrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1frk6d8</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mystery nail stickers </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8cyyndmalrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1frk66h</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Took a stab at tortoise shell press-on nails, now that we’re officially in autumn territory!</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldaqc92lalrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1frk30u</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I love doing my nails 💅🏼💕</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frk30u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1frjhzi</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Nail salon struggles and my new obsession 🌸</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c94acyg95lrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1frjftu</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like my new nails </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hve9gshs4lrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1frjbk0</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few newbie questions </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frjbk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1frj8ws</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>My nails are short, but I love the designs!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqykyr673lrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1frizj7</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Gatita gánster 🌈- by kitecosmicnails</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fem6cc441lrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1frixxj</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is so hard to find medium length oval nails (not almond) </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frixxj/why_is_so_hard_to_find_medium_length_oval_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1frix16</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Philly Nail Tech</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frix16/philly_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1frivq8</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Your Press on nail sizes</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1frivq8/your_press_on_nail_sizes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1frim7c</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Can I file these “ballerina” nails at home?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbq1p9z3ykrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1fri20k</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>first time getting acrylics in a year🩷</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c39liemjtkrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1frhw2x</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>obsessed 🥹💘</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frhw2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1frh8ce</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sharing my birthday nails I did! </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frh8ce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1frh0bk</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Chrome luv for when I go see Kaytranada next week :p</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frh0bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1frgu6c</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>September nails!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frgu6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1frgn77</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Two Loves. 📚 &amp; 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frgn77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1frgdkz</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Complete newbie, please help me understand my options</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w948hr6xfkrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1frgae7</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frgae7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1frg2gs</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Are you kitten me right meow?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2aynhjidkrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1frftuq</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>october nails! (from russian nails nyc!) 💜✨</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frftuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1frfhr5</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>New set its giving vampire</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubgzekfm8krd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1frey2h</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Chrome Green Aura</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dnj18hir3krd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1freck8</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥳</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/737dlz3byjrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1frebsf</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween but make it cutesy! </t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ky0ia64yjrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1fre60g</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My previous nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jppbe74nwjrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1fre2es</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>I’m a Beginner</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fre2es</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1frd3jf</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Catsronaut Nails</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frd3jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1frcq45</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seashell to blob </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3r7sgheijrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1frbhuo</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Been very happy with my recent nail designs</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frbhuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1frbd0t</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Matte flowers</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcxvj7bt1jrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1frzeht</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Bright and polished</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frzeht/bright_and_polished/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1frzb15</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>This Green Polish Is Probably Over A Decade Old!</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frzb15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1frxl4l</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Drunk Fairy Polish Controversy </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frxl4l/drunk_fairy_polish_controversy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1frw5jp</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Dollar Tree haul</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv8hexp3cord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1frvgnj</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got into polish… apparently lots of the gorgeous polishes are discontinued? 😭 </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frvgnj/just_got_into_polish_apparently_lots_of_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1frvdwx</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>New to nails!!</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frvdwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1fruy1o</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>An odd fall combo I’m calling poison caramel apple 🍎💚🍂</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fruy1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1frueiu</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Modern dupe for this vintage red glitter? </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8td0sbotnrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1frud9r</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Matte Fall Colors Give Me Life 💅🍂</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frud9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1fru6ff</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Monarch - Psycho</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fru6ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1fru0kf</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer - Fun With Foliage 🍁</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fru0kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1frth7o</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>It's my turn for the psilocybin train</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pq3bjqleknrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1frsskk</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>The last summery set 🌊</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sto8wv9kdnrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1frshr9</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Back with X-Men nails: Gambit ♣️♥ (+ glow in the dark)</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frshr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1frro43</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>It’s Just a Phase</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frro43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1frrndb</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>This fall mani is so good I had to refresh it 🔥💅✨️</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/94prvtwh2nrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1frrkep</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Call a Halloween mani (but not for me)</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frrkep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1frqscd</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail color to go with this color dress </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tp1746mumrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1frqdvo</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Holo Taco’s Inkwell</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frqdvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1frpy6u</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Are Mooncat's bottles still breaking?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frpy6u/are_mooncats_bottles_still_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1frpxp6</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>I rarely wear pinks, but this shade was too juicy not to!</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3han8r0nmrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1frpinu</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue and pink opal nails 😻 which would you rock? </t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frpinu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1frp720</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Tilted by ILNP</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4i745x1bgmrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1frok0u</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Couldn't decide which one to wear, so I did both 💜</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvfk9l9mamrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1frohmm</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Cosy weekend nails</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrir5bq5amrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1frobu8</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally realized why the polish on my fingernails chip in a few days whereas the ones on my toenails last for weeks without any chips </t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frobu8/i_finally_realized_why_the_polish_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1frnvq5</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Bill is amazing ✨</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frnvq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1frnmwf</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>How to fix this?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fzbhprx2mrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1frn3q9</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Now Go and Don't Look Back</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frn3q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1frmi6f</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Help for a Clueless Husband</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frmi6f/help_for_a_clueless_husband/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1frmgl0</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>PPU Haul + current mani</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frmgl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1frlt2y</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>I'm babysitting my brother in law's beefy gaming PC while he moves, so I'm going to be chopping my nails down to play BG3 and write fanfic :') I'm excited but I'm gonna miss my long nails, too. Help me celebrate by sharing some pics in the comments of your favorite manicures you've had!</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frlt2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1frlt1c</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Freshly bitten</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frlt1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1frlnuc</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Nail layers flaking?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frlnuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1frl5ej</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Liquid Fire</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8bw5xwjilrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1frl1q7</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>ILNP- Autumn 🍁🍂🍃</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frl1q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1frkf4l</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Nailed It! Moonblast</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frkf4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1frk92s</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Week 2 of nail polish jail</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnlgrxntalrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1frk593</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Order your preferred nail polish effects from favorite to least favorite!</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frk593/order_your_preferred_nail_polish_effects_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1frk3ut</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>OPI Glazed and Amused</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q75sn73alrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1frk2qm</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Do i need the essie gel top coat for its 2 part gel couture line or can i use my revlon top coat</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvp2nvut9lrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1frjwub</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Gf's first poly gel extension</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvm3p0gj8lrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1frjpgp</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>ILNP Birefringence is giving me life</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zrlie4vx6lrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1frjd44</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>She knows she glows</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frjd44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1frh67o</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sharing my birthday nails I did! </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frh67o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1frh5fu</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>When is the best time to buy ILNP?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1frh5fu/when_is_the_best_time_to_buy_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1frgkxk</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>I’ve got a dead ringer for Dead Ringer</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frgkxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1fr8xhd</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>New to nails and based in the UK - advice on base, top, best brands please!</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fr8xhd/new_to_nails_and_based_in_the_uk_advice_on_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1frfjwh</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wowzas! </t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32q56dv49krd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1frfczg</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>First time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frfczg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1frfakd</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Clionadh Psilocybin + Cephalopod</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmn0erlv6krd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1frey7p</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sep 24 PPU haul </t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dludubpt3krd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1fregx0</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saw some boobies in my garden this morning. </t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fregx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1fre20y</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Uneven nails</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fre20y/uneven_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1frds0q</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>The living usually won’t see the  dead</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frds0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1fra70x</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Removing holo polish?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fra70x/removing_holo_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1fr9phu</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>How Essie releases new collections in Canada 😐 not a new color in sight</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fr9phu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1frz5xb</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>My new favourite set</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frz5xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1frw7ou</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Paul Frank/ planned pines themed press ons! </t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vz4voo3ucord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1frvhx1</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My acrylic nails </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owllymr25ord1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1frujp6</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Used my new makeup products as nail inspo 🍓🎀</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zij1dr65vnrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1frub42</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>3D hand sculpted hanging cat for Halloween 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frub42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1frttts</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Did a new set this week</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48pw7moznnrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1frtac5</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where My Dotticure Fiends? </t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84vgnkmginrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1frru5q</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Spooky season set #2! I promised you more!🧡🖤🎃🍁</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ultja994nrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1frqjnu</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>My nail tech killed it with these dessert nails (@the_polish_parlour on insta)</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frqjnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1frpds3</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>First ever set I did 🤭</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qckyo282imrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1frpdbr</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Koi fish nails on my client </t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frpdbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1fro7ed</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Black and white floral set</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fro7ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1frmsf0</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>First attempt at Gel-X</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frmsf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1frmh74</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>XL barbie nails</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbtuocuetlrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1frl932</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Björk album art </t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frl932</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1frl0qv</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>nails for mom</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yqmyblihlrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1frkxx5</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the perfect tone </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19tiqb4uglrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1frk4cw</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nanananananaaaaa BAT NAILS! </t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p37k1k07alrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1frjp3a</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Castronaut Nails by Ryn at Soirée Beauty in Columbus</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1frjp3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1frid7p</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Early spooky set</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p26770h3wkrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1fre45e</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing French tips. How’d I do? </t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/098p7sm5wjrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1fraukd</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Some more retro fall vibe</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk5o3f37vird1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1fra8s4</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Finally finished!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fra8s4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>